<commit_message>
Add more lines, notably lots of caro kann
</commit_message>
<xml_diff>
--- a/Openings.xlsx
+++ b/Openings.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="202">
   <si>
     <t>Variation</t>
   </si>
@@ -291,6 +291,120 @@
     <t>1. e4 c6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Bf5 5. Ng3 Bg6 6. h4 h6 7. Nf3 Nd7 8. h5 Bh7 9. Bd3 Bxd3 10. Qxd3 e6 11. Bf4 Ngf6 12. O-O-O Qa5 13. Kb1 Be7 14. Ne5 O-O 15. Nxd7 Nxd7 16. Ne4 Nf6 17. g4 Rad8</t>
   </si>
   <si>
+    <t>1. e4 c6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Bf5 5. Ng3 Bg6 6. h4 h6 7. Nf3 Nd7 8. h5 Bh7 9. Bd3 Bxd3 10. Qxd3 e6 11. Bd2 Ngf6 12. O-O-O Be7 13. Qe2 O-O 14. Ne5 c5 15. dxc5 Nxc5 16. Kb1 Qc7 17. Bc3 Rfd8</t>
+  </si>
+  <si>
+    <t>4... Bf5 Variation</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Bf5 5. Ng3 Bg6 6. h4 h6 7. Nf3 Nd7 8. Bd3 Bxd3 9. Qxd3 Qc7 10. Bd2 Ngf6 11. O-O-O e6 12. Kb1 O-O-O</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Bf5 5. Ng3 Bg6 6. h4 h6 7. Nf3 Nf6 8. Ne5 Bh7 9. Bd3 Bxd3 10. Qxd3 e6 11. Bd2 Nbd7 12. f4 Be7</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Bf5 5. Ng3 Bg6 6. h4 h6 7. f4 e6 8. Nf3 Nd7 9. h5 Bh7 10. Bd3 Bxd3 11. Qxd3 Qc7 12. Bd2 Ngf6</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Bf5 5. Ng3 Bg6 6. Bc4 e6 7. N1e2 Nf6 8. O-O Bd6 9. f4 Qe7 10. Bd3 Bxd3 11. Qxd3 g6 12. f5 gxf5</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Bf5 5. Ng3 Bg6 6. Nf3 Nd7 7. Bd3 e6 8. O-O Ngf6 9. c4 Bd6 10. b3 O-O 11. Bb2 c5 12. Bxg6 hxg6</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Bf5 5. Ng3 Bg6 6. N1e2 Nf6 7. Nf4 e5 8. Nxg6 hxg6 9. dxe5 Qa5+ 10. Bd2 Qxe5+ 11. Qe2 Qxe2+ 12. Bxe2 Nbd7</t>
+  </si>
+  <si>
+    <t>Main Line 4... Nd7</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Nd7 5. Bd3 Ngf6 6. Ng5 e6 7. N1f3 Bd6 8. Qe2 h6 9. Ne4 Nxe4 10. Qxe4 Nf6 11. Qe2 Qc7 12. Bd2 b6 13. O-O-O Bb7</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Nd7 5. Bd3 Ngf6 6. Ng5 e6 7. N1f3 Bd6 8. Qe2 h6 9. Ne4 Nxe4 10. Qxe4 Qc7 11. O-O b6 12. Qg4 Kf8 13. b3 Bb7</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Nd7 5. Bd3 Ngf6 6. Ng5 e6 7. N1f3 h6 8. Nxe6 fxe6 9. Bg6+ Ke7 10. Bf4 Qa5+ 11. c3 Kd8 12. O-O Be7 13. Re1 Nf8</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Nd7 5. Ng5 Ndf6 6. N1f3 Bg4 7. h3 Bxf3 8. Nxf3 e6 9. g3 Bd6 10. Bg2 Ne7 11. O-O O-O 12. Qe2 Qc7 13. c4 b6</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Nd7 5. Nf3 Ngf6 6. Ng3 e6 7. Bd3 c5 8. O-O cxd4 9. Nxd4 Bc5 10. c3 O-O 11. Bd2 Re8 12. Bg5 a6 13. Qf3 Bxd4</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Nd7 5. Nf3 Ngf6 6. Ng3 c5 7. dxc5 e6 8. b4 b6 9. Be2 bxc5 10. b5 Bb7 11. O-O Qc7 12. c4 Bd6 13. Qd2 Ne5</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Nd7 5. Nf3 Ngf6 6. Nxf6+ Nxf6 7. Ne5 Be6 8. Be2 g6 9. O-O Bg7 10. c4 O-O 11. Be3 Ne4 12. f4 Nd6 13. b3 Qc7</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Nd7 5. Nf3 Ngf6 6. Nxf6+ Nxf6 7. Ne5 Nd7 8. Bf4 Nxe5 9. Bxe5 Qd5 10. c4 Qa5+ 11. Qd2 Qxd2+ 12. Kxd2 Bf5 13. Bd3 Bxd3</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Nd7 5. Bc4 Ngf6 6. Ng5 e6 7. Qe2 Nb6 8. Bb3 h6 9. N5f3 a5 10. c3 c5 11. a3 Qc7 12. Nh3 Bd7 13. O-O cxd4</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Nd7 5. Bc4 Ngf6 6. Ng5 e6 7. Qe2 Nb6 8. Bb3 h6 9. N5f3 c5 10. Bf4 Nbd5 11. Be5 Qa5+ 12. Nd2 b5 13. dxc5 Bxc5</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Nd7 5. Bc4 Ngf6 6. Ng5 e6 7. Qe2 Nb6 8. Bd3 h6 9. N5f3 c5 10. dxc5 Bxc5 11. Ne5 Nbd7 12. Ngf3 Qc7 13. O-O O-O</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Nd7 5. Bc4 Ngf6 6. Nxf6+ Nxf6 7. c3 Qc7 8. Qb3 e6 9. Nf3 Bd6 10. Bg5 Nd5 11. O-O b6 12. Rfe1 O-O 13. Qc2 h6</t>
+  </si>
+  <si>
+    <t>Advance Variation</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. e5 Bf5 4. Nf3 e6 5. Be2 Ne7 6. O-O Nd7 7. Nh4 Bg6 8. Nd2 c5 9. c3 Nc6 10. Nxg6 hxg6 11. Nf3 cxd4 12. cxd4 Be7</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. e5 Bf5 4. Nf3 e6 5. Be2 c5 6. O-O Nc6 7. c3 Bg4 8. Nbd2 cxd4 9. cxd4 Nge7 10. a3 Nf5 11. b4 Be7 12. h3 Bxf3</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. e5 Bf5 4. Nc3 e6 5. g4 Bg6 6. Nge2 c5 7. h4 h6 8. Be3 Qb6 9. f4 Nc6 10. f5 Bh7 11. Qd2 O-O-O 12. O-O-O c4</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. e5 Bf5 4. Nc3 Qb6 5. g4 Bd7 6. Na4 Qc7 7. Nc5 e6 8. Nxd7 Nxd7 9. f4 c5 10. c3 Ne7 11. Nf3 h5 12. gxh5 Nf5</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. e5 Bf5 4. h4 h5 5. c4 e6 6. Nc3 dxc4 7. Bxc4 Nd7 8. Bg5 Be7 9. Qd2 Qa5 10. Nge2 O-O-O 11. Qe3 Bxg5 12. hxg5 Nb6</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. e5 c5 4. dxc5 Nc6 5. Bb5 e6 6. Be3 Ne7 7. c3 Nf5 8. Bd4 Bd7 9. Bxc6 Bxc6 10. Nf3 Nxd4 11. Qxd4 a5 12. b4 axb4</t>
+  </si>
+  <si>
+    <t>Two Knights' Variation</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. Nc3 d5 3. Nf3 Bg4 4. h3 Bxf3 5. Qxf3 Nf6 6. d3 e6 7. Bd2 Nbd7 8. g4 Bb4 9. g5 Ng8 10. h4 d4 11. Nb1 Qb6</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. Nc3 d5 3. Nf3 Bg4 4. h3 Bxf3 5. Qxf3 Nf6 6. d3 e6 7. g3 Bb4 8. Bd2 d4 9. Nb1 Qb6 10. b3 a5 11. a3 Bxd2+</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. Nc3 d5 3. Nf3 Bg4 4. h3 Bxf3 5. Qxf3 e6 6. d4 dxe4 7. Nxe4 Nf6 8. Bd3 Qxd4 9. c3 Qd8 10. O-O Nbd7 11. Bf4 Nxe4</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. Nc3 d5 3. Nf3 Bg4 4. h3 Bh5 5. exd5 cxd5 6. Bb5+ Nc6 7. g4 Bg6 8. Ne5 Rc8 9. d4 e6 10. Qe2 Bb4 11. h4 Ne7</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. Nc3 d5 3. Nf3 Nf6 4. e5 Ne4 5. Ne2 Bg4 6. Nfg1 Bxe2 7. Bxe2 e6 8. d3 Nc5 9. Nf3 Ncd7 10. O-O c5 11. c3 Nc6</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. Nc3 d5 3. Nf3 dxe4 4. Nxe4 Nd7 5. Bc4 Ngf6 6. Neg5 e6 7. Qe2 Nd5 8. d4 h6 9. Ne4 Be7 10. O-O O-O 11. a4 a5</t>
+  </si>
+  <si>
+    <t>Exchange Variation</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. exd5 cxd5 4. Bd3 Nc6 5. c3 Nf6 6. Bf4 Bg4 7. Qb3 Qd7 8. Nd2 e6 9. Ngf3 Bxf3 10. Nxf3 Bd6</t>
+  </si>
+  <si>
+    <t>1. e4 c6 2. d4 d5 3. exd5 cxd5 4. Bd3 Nc6 5. c3 Qc7 6. Ne2 Bg4 7. f3 Bd7 8. Na3 a6 9. Nc2 e6 10. Bf4 Bd6</t>
+  </si>
+  <si>
     <t>Classical (Cordel) Defence</t>
   </si>
   <si>
@@ -321,9 +435,6 @@
     <t>1. e4 e5 2. Nf3 Nc6 3. Bb5 Bc5 4. c3 Nge7 5. O-O Bb6 6. d4 exd4 7. cxd4 d5 8. exd5 Nxd5 9. Re1+ Be6 10. Bg5 Qd6</t>
   </si>
   <si>
-    <t>Exchange Variation</t>
-  </si>
-  <si>
     <t>1. e4 e5 2. Nf3 Nc6 3. Bb5 a6 4. Bxc6 dxc6 5. O-O f6 6. d4 Bg4 7. dxe5 Qxd1 8. Rxd1 fxe5 9. Rd3 Bd6 10. Nbd2 Nf6 11. b3 O-O-O 12. Bb2 Rhe8</t>
   </si>
   <si>
@@ -342,6 +453,48 @@
     <t>1. e4 e5 2. Nf3 Nc6 3. Bb5 a6 4. Bxc6 dxc6 5. d4 exd4 6. Qxd4 Qxd4 7. Nxd4 Bd7 8. Be3 O-O-O 9. Nd2 Ne7 10. O-O-O Re8 11. Rhe1 Ng6 12. Ne2 Bd6</t>
   </si>
   <si>
+    <t>Modern Steinitz Defence</t>
+  </si>
+  <si>
+    <t>1. e4 e5 2. Nf3 Nc6 3. Bb5 a6 4. Ba4 d6 5. c3 Bd7 6. d4 g6 7. O-O Bg7 8. Be3 Nf6 9. Nbd2 O-O 10. h3 Qe8 11. Bxc6 Bxc6 12. dxe5 Nxe4 13. Nxe4 Bxe4</t>
+  </si>
+  <si>
+    <t>1. e4 e5 2. Nf3 Nc6 3. Bb5 a6 4. Ba4 d6 5. c3 Bd7 6. d4 g6 7. O-O Bg7 8. d5 Nce7 9. Bxd7+ Qxd7 10. c4 h6 11. Nc3 f5 12. Ne1 Nf6 13. f3 O-O</t>
+  </si>
+  <si>
+    <t>1. e4 e5 2. Nf3 Nc6 3. Bb5 a6 4. Ba4 d6 5. c3 Bd7 6. d4 Nge7 7. O-O Ng6 8. d5 Nb8 9. c4 Be7 10. Nc3 h6 11. b4 a5 12. a3 O-O 13. Be3 Bxa4</t>
+  </si>
+  <si>
+    <t>1. e4 e5 2. Nf3 Nc6 3. Bb5 a6 4. Ba4 d6 5. c3 Bd7 6. d4 Nf6 7. O-O Qe7 8. Re1 g6 9. Nbd2 Bg7 10. Nf1 O-O 11. Bg5 h6 12. Bh4 Qe8 13. Bc2 Nh5</t>
+  </si>
+  <si>
+    <t>Modern Steinitz Defence, Siesta Variation</t>
+  </si>
+  <si>
+    <t>1. e4 e5 2. Nf3 Nc6 3. Bb5 a6 4. Ba4 d6 5. c3 f5 6. exf5 Bxf5 7. O-O Bd3 8. Re1 Be7 9. Bc2 Bxc2 10. Qxc2 Nf6 11. d4 O-O 12. d5 e4 13. Ng5 Ne5</t>
+  </si>
+  <si>
+    <t>1. e4 e5 2. Nf3 Nc6 3. Bb5 a6 4. Ba4 d6 5. c3 f5 6. exf5 Bxf5 7. d4 e4 8. Ng5 d5 9. f3 h6 10. fxe4 hxg5 11. exf5 Bd6 12. Qf3 g4 13. Qxg4 Nf6 14. Qf3</t>
+  </si>
+  <si>
+    <t>1. e4 e5 2. Nf3 Nc6 3. Bb5 a6 4. Ba4 d6 5. O-O Bg4 6. h3 h5 7. d4 b5 8. Bb3 Nxd4 9. hxg4 Nxb3 10. axb3 hxg4 11. Ng5 Qd7 12. c4 Rb8</t>
+  </si>
+  <si>
+    <t>1. e4 e5 2. Nf3 Nc6 3. Bb5 a6 4. Ba4 d6 5. O-O Bd7 6. d4 b5 7. Bb3 Nxd4 8. Nxd4 exd4 9. c3 dxc3 10. Qh5 Qe7 11. Nxc3 Nf6 12. Qd1 c6</t>
+  </si>
+  <si>
+    <t>1. e4 e5 2. Nf3 Nc6 3. Bb5 a6 4. Ba4 d6 5. Bxc6+ bxc6 6. d4 f6 7. Be3 Ne7 8. Nc3 Ng6 9. Qe2 Be7 10. O-O-O Be6 11. h4 h5 12. dxe5 fxe5</t>
+  </si>
+  <si>
+    <t>1. e4 e5 2. Nf3 Nc6 3. Bb5 a6 4. Ba4 d6 5. Bxc6+ bxc6 6. d4 exd4 7. Qxd4 c5 8. Qd3 g6 9. Nc3 Bg7 10. Bf4 Ne7 11. Qd2 O-O 12. Bh6 Bg4</t>
+  </si>
+  <si>
+    <t>1. e4 e5 2. Nf3 Nc6 3. Bb5 a6 4. Ba4 d6 5. c4 Bd7 6. Nc3 g6 7. d4 exd4 8. Nxd4 Bg7 9. Be3 Nge7 10. O-O O-O 11. h3 Nxd4 12. Bxd7 Ne2+</t>
+  </si>
+  <si>
+    <t>1. e4 e5 2. Nf3 Nc6 3. Bb5 a6 4. Ba4 d6 5. d4 b5 6. Bb3 Nxd4 7. Nxd4 exd4 8. Bd5 Rb8 9. Bc6+ Bd7 10. Bxd7+ Qxd7 11. Qxd4 Nf6 12. Nc3 Be7</t>
+  </si>
+  <si>
     <t>Orthodox Variation</t>
   </si>
   <si>
@@ -415,9 +568,6 @@
   </si>
   <si>
     <t>1. d4 d5 2. c4 e6 3. Nc3 Nf6 4. Nf3 c5 5. cxd5 Nxd5 6. g3 Nc6 7. Bg2 Be7 8. O-O O-O 9. Nxd5 exd5 10. dxc5 Bxc5 11. Bg5 Qb6 12. Ne1 h6</t>
-  </si>
-  <si>
-    <t>Advance Variation</t>
   </si>
   <si>
     <t>1. e4 e6 2. d4 d5 3. e5 c5 4. c3 Nc6 5. Nf3 Qb6 6. Be2 cxd4 7. cxd4 Nh6 8. Nc3 Nf5 9. Na4 Bb4+ 10. Bd2 Qa5 11. Bc3 b5 12. a3 Bxc3+</t>
@@ -1371,6 +1521,270 @@
         <v>84</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1386,7 +1800,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="30.57"/>
+    <col customWidth="1" min="1" max="1" width="36.57"/>
     <col customWidth="1" min="2" max="2" width="161.71"/>
   </cols>
   <sheetData>
@@ -1400,114 +1814,210 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>86</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>88</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>90</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>91</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>92</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>93</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>96</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>97</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>98</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>99</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>100</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>101</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1539,186 +2049,186 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>102</v>
+        <v>153</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>103</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>153</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>104</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>102</v>
+        <v>153</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>105</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>102</v>
+        <v>153</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>106</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>102</v>
+        <v>153</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>107</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>102</v>
+        <v>153</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>108</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>102</v>
+        <v>153</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>109</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>102</v>
+        <v>153</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>110</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>111</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>112</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>113</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>114</v>
+        <v>165</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>115</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>114</v>
+        <v>165</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>116</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>114</v>
+        <v>165</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>117</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>114</v>
+        <v>165</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>118</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>114</v>
+        <v>165</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>119</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>114</v>
+        <v>165</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>120</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>114</v>
+        <v>165</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>121</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>114</v>
+        <v>165</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>122</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>114</v>
+        <v>165</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>123</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>114</v>
+        <v>165</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>124</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>114</v>
+        <v>165</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>125</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>114</v>
+        <v>165</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>126</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25">
@@ -1756,42 +2266,42 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>128</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>129</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>130</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>131</v>
+        <v>181</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>132</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>133</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7">
@@ -1863,50 +2373,50 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>135</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>136</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>137</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>138</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>139</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>140</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -1938,66 +2448,66 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>141</v>
+        <v>191</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>142</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>141</v>
+        <v>191</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>143</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>141</v>
+        <v>191</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>144</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>145</v>
+        <v>195</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>146</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>145</v>
+        <v>195</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>147</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>148</v>
+        <v>198</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>149</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>148</v>
+        <v>198</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>150</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>148</v>
+        <v>198</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>151</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Petrov and french defence
</commit_message>
<xml_diff>
--- a/Openings.xlsx
+++ b/Openings.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sicillian Defence" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Sicilian Defence" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Caro-Kann Defence" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="Ruy Lopez" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="Queen's Gambit Declined" sheetId="4" r:id="rId7"/>
@@ -11,7 +11,9 @@
     <sheet state="visible" name="Tarrasch Defence" sheetId="6" r:id="rId9"/>
     <sheet state="visible" name="King's Indian Defence" sheetId="7" r:id="rId10"/>
     <sheet state="visible" name="Catalan Opening" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="Template" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="London System" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="Petrov's Defence" sheetId="10" r:id="rId13"/>
+    <sheet state="visible" name="Template" sheetId="11" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="299">
   <si>
     <t>Variation</t>
   </si>
@@ -589,6 +591,102 @@
     <t>1. e4 e6 2. d4 d5 3. exd5 exd5 4. Bd3 Bd6 5. c3 Nc6 6. Nf3 Nge7 7. O-O Bg4 8. Re1 Qd7 9. Nbd2 O-O 10. h3 Bf5</t>
   </si>
   <si>
+    <t>1. e4 e6 2. d4 d5 3. e5 c5 4. c3 Nc6 5. Nf3 Bd7 6. Be2 Nge7 7. O-O cxd4 8. cxd4 Nf5 9. Nc3 Rc8 10. a3 a6 11. Be3 Be7 12. Bd3 Nxe3</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. e5 c5 4. c3 Nc6 5. Nf3 Nge7 6. Na3 cxd4 7. cxd4 Nf5 8. Nc2 Qb6 9. Bd3 Bb4+ 10. Kf1 Be7 11. h4 Bd7 12. g4 Nh6</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. e5 c5 4. Nf3 cxd4 5. Bd3 Nc6 6. O-O Nge7 7. Bf4 Ng6 8. Bg3 Be7 9. Nbd2 f5 10. exf6 gxf6 11. Nh4 f5 12. Nxg6 hxg6</t>
+  </si>
+  <si>
+    <t>Classical Variation</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. Nc3 Nf6 4. Bg5 Be7 5. e5 Nfd7 6. Bxe7 Qxe7 7. f4 O-O 8. Nf3 c5 9. Qd2 Nc6 10. O-O-O Nb6 11. Qe3 cxd4 12. Nxd4 Nxd4 13. Rxd4 Bd7 14. h4</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. Nc3 Nf6 4. Bg5 Be7 5. e5 Nfd7 6. Bxe7 Qxe7 7. f4 O-O 8. Nf3 c5 9. Qd2 Nc6 10. O-O-O Nb6 11. dxc5 Qxc5 12. Bd3 Bd7 13. Kb1 Rac8 14. Bxh7+ Kxh7</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. Nc3 Nf6 4. Bg5 Be7 5. e5 Nfd7 6. Bxe7 Qxe7 7. f4 O-O 8. Nf3 c5 9. dxc5 Nc6 10. Bd3 f6 11. exf6 Qxf6 12. g3 Nxc5 13. O-O Bd7 14. Qd2 Nxd3</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. Nc3 Nf6 4. Bg5 Be7 5. e5 Nfd7 6. Bxe7 Qxe7 7. Bd3 O-O 8. Nce2 c5 9. c3 f6 10. f4 fxe5 11. fxe5 cxd4 12. Nxd4 Nxe5 13. Bxh7+ Kxh7 14. Qh5+ Kg8</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. Nc3 Nf6 4. Bg5 Be7 5. e5 Nfd7 6. h4 Bxg5 7. hxg5 Qxg5 8. Qd3 g6 9. Nf3 Qe7 10. O-O-O Nc6 11. Qe3 Nb6 12. g4 Bd7 13. Rh6 O-O-O 14. g5 Na5</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. Nc3 Nf6 4. Bg5 Be7 5. e5 Nfd7 6. h4 c5 7. Bxe7 Kxe7 8. f4 Qb6 9. Na4 Qc6 10. Nxc5 Nxc5 11. dxc5 Qxc5 12. Qd2 Nc6 13. O-O-O Bd7 14. Kb1</t>
+  </si>
+  <si>
+    <t>MacCutcheon Variation</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. Nc3 Nf6 4. Bg5 Bb4 5. e5 h6 6. Bd2 Bxc3 7. bxc3 Ne4 8. Qg4 g6 9. Bd3 Nxd2 10. Kxd2 c5 11. Nf3 Nc6 12. Qf4 Qa5 13. dxc5 Qxc5</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. Nc3 Nf6 4. Bg5 Bb4 5. e5 h6 6. Bd2 Bxc3 7. bxc3 Ne4 8. Qg4 Kf8 9. Bd3 Nxd2 10. Kxd2 c5 11. Nf3 Nc6 12. dxc5 Qa5 13. Qf4 Qxc5</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. Nc3 Nf6 4. Bg5 Bb4 5. e5 h6 6. Bd2 Bxc3 7. Bxc3 Ne4 8. Bb4 c5 9. Bxc5 Nxc5 10. dxc5 Nd7 11. Qd4 Qc7 12. Nf3 Nxc5 13. Bd3 Bd7</t>
+  </si>
+  <si>
+    <t>Burn's Variation</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. Nc3 Nf6 4. Bg5 dxe4 5. Nxe4 Be7 6. Bxf6 Bxf6 7. Nf3 O-O 8. Qd2 b6 9. Nxf6+ Qxf6 10. Bd3 Bb7 11. Ng5 h6 12. Nh7 Qxd4 13. Nxf8 Kxf8</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. Nc3 Nf6 4. Bg5 dxe4 5. Nxe4 Be7 6. Bxf6 gxf6 7. Nf3 b6 8. Bc4 Bb7 9. Qe2 c6 10. O-O-O Qc7 11. Rhe1 Nd7 12. Kb1 O-O-O 13. Ba6 Bxa6</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. Nc3 Nf6 4. Bg5 dxe4 5. Nxe4 Nbd7 6. Nf3 Be7 7. Nxf6+ Bxf6 8. h4 h6 9. Bxf6 Qxf6 10. Bc4 O-O 11. Qe2 c5 12. O-O-O cxd4 13. Rxd4 e5</t>
+  </si>
+  <si>
+    <t>Rubinstein Variation</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Nd7 5. Nf3 Ngf6 6. Nxf6+ Nxf6 7. Bg5 h6 8. Bxf6 Qxf6 9. Bb5+ c6 10. Bd3 Bd7 11. c3 Bd6 12. Qe2 c5</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Nd7 5. Nf3 Ngf6 6. Nxf6+ Nxf6 7. Bg5 c5 8. Bb5+ Bd7 9. Bxd7+ Qxd7 10. Qe2 Be7 11. O-O-O O-O 12. dxc5 Qc6</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Nd7 5. Nf3 Ngf6 6. Nxf6+ Nxf6 7. Bd3 c5 8. dxc5 Bxc5 9. Qe2 Qc7 10. Bd2 O-O 11. O-O-O b6 12. Ne5 Bb7</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Nd7 5. Nf3 Ngf6 6. Nxf6+ Nxf6 7. Bd3 Be7 8. Qe2 O-O 9. Bg5 c5 10. dxc5 Qa5+ 11. c3 Qxc5 12. O-O-O g6</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Nd7 5. Nf3 Be7 6. Bd3 Ngf6 7. Qe2 O-O 8. O-O b6 9. Nxf6+ Nxf6 10. c4 Bb7 11. Rd1 Qe8 12. Bd2 Rd8</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. Nc3 dxe4 4. Nxe4 Bd7 5. Nf3 Bc6 6. Bd3 Nd7 7. O-O Ngf6 8. Ng3 Be7 9. b3 O-O 10. Bb2 Bxf3 11. Qxf3 c6 12. c4 Re8</t>
+  </si>
+  <si>
+    <t>Steinitz Variation</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. Nc3 Nf6 4. e5 Nfd7 5. f4 c5 6. Nf3 Nc6 7. Be3 Qb6 8. Na4 Qa5+ 9. c3 cxd4 10. b4 Nxb4 11. cxb4 Bxb4+ 12. Bd2 Bxd2+ 13. Nxd2 b6</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. Nc3 Nf6 4. e5 Nfd7 5. f4 c5 6. Nf3 Nc6 7. Be3 Qb6 8. Na4 Qa5+ 9. c3 c4 10. b4 Qc7 11. Be2 Be7 12. O-O O-O 13. g4 b5</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. Nc3 Nf6 4. e5 Nfd7 5. f4 c5 6. Nf3 Nc6 7. Be3 cxd4 8. Nxd4 Qb6 9. Qd2 Qxb2 10. Rb1 Qa3 11. Bb5 Nxd4 12. Bxd4 Bb4 13. O-O a6</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. Nc3 Nf6 4. e5 Nfd7 5. f4 c5 6. Nf3 Nc6 7. Be3 cxd4 8. Nxd4 Bc5 9. Qd2 O-O 10. O-O-O a6 11. h4 Nxd4 12. Bxd4 b5 13. Kb1 Qc7</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. Nc3 Nf6 4. e5 Nfd7 5. f4 c5 6. Nf3 Nc6 7. Be3 a6 8. Qd2 b5 9. dxc5 Bxc5 10. Bxc5 Nxc5 11. Qf2 Qb6 12. Bd3 Rb8 13. O-O Na4</t>
+  </si>
+  <si>
+    <t>1. e4 e6 2. d4 d5 3. Nc3 Nf6 4. e5 Nfd7 5. Nf3 c5 6. dxc5 Nc6 7. Bf4 Bxc5 8. Bd3 f6 9. exf6 Nxf6 10. O-O O-O 11. Ne5 Bd7 12. Nxc6 Bxc6 13. Qe2 Qe7</t>
+  </si>
+  <si>
     <t>Tarrasch Defence</t>
   </si>
   <si>
@@ -791,6 +889,51 @@
   </si>
   <si>
     <t>1. d4 Nf6 2. c4 e6 3. g3 d5 4. Bg2 Be7 5. Nf3 O-O 6. O-O Na6 7. Nc3 c5 8. cxd5 exd5 9. dxc5 Nxc5 10. Be3 Nce4 11. Rc1 Be6 12. Nd4 Bd7 13. Nxe4 dxe4</t>
+  </si>
+  <si>
+    <t>London System</t>
+  </si>
+  <si>
+    <t>1. d4 d5 2. Bf4 Nf6 3. Nf3 c5 4. e3 Nc6 5. c3 e6 6. Nbd2 Bd6 7. Bg3 O-O 8. Bd3 b6 9. Ne5 Bb7 10. f4 Ne7 11. Qf3 Nf5 12. Bf2 Be7 13. O-O Nd6 14. Rad1 c4</t>
+  </si>
+  <si>
+    <t>Petrov's Defence</t>
+  </si>
+  <si>
+    <t>1. e4 e5 2. Nf3 Nf6 3. Nxe5 d6 4. Nf3 Nxe4 5. d4 d5 6. Bd3 Be7 7. O-O Nc6 8. c4 Nb4 9. Be2 O-O 10. Nc3 Be6 11. Be3 Bf5 12. Qb3 c6</t>
+  </si>
+  <si>
+    <t>1. e4 e5 2. Nf3 Nf6 3. Nxe5 d6 4. Nf3 Nxe4 5. d4 d5 6. Bd3 Be7 7. O-O Nc6 8. Re1 Bg4 9. c3 f5 10. Qb3 O-O 11. Nbd2 Kh8 12. Qxb7 Rf6</t>
+  </si>
+  <si>
+    <t>1. e4 e5 2. Nf3 Nf6 3. Nxe5 d6 4. Nf3 Nxe4 5. d4 d5 6. Bd3 Nc6 7. O-O Bg4 8. c4 Nf6 9. cxd5 Bxf3 10. Qxf3 Qxd5 11. Qe2+ Be7 12. Bb5 Qd6</t>
+  </si>
+  <si>
+    <t>1. e4 e5 2. Nf3 Nf6 3. Nxe5 d6 4. Nf3 Nxe4 5. d4 d5 6. Bd3 Bd6 7. O-O O-O 8. c4 c6 9. cxd5 cxd5 10. Nc3 Nxc3 11. bxc3 Bg4 12. Rb1 b6</t>
+  </si>
+  <si>
+    <t>1. e4 e5 2. Nf3 Nf6 3. Nxe5 d6 4. Nf3 Nxe4 5. d4 d5 6. Bd3 Bd6 7. O-O O-O 8. c4 c6 9. Qc2 Na6 10. a3 f5 11. Nc3 Nc7 12. b4 Nxc3</t>
+  </si>
+  <si>
+    <t>1. e4 e5 2. Nf3 Nf6 3. Nxe5 d6 4. Nf3 Nxe4 5. d4 Be7 6. Bd3 Nf6 7. h3 O-O 8. O-O Re8 9. c4 Nc6 10. Nc3 h6 11. Re1 Bf8 12. Rxe8 Qxe8</t>
+  </si>
+  <si>
+    <t>1. e4 e5 2. Nf3 Nf6 3. Nxe5 d6 4. Nf3 Nxe4 5. Qe2 Qe7 6. d3 Nf6 7. Bg5 Qxe2+ 8. Bxe2 Be7 9. Nc3 c6 10. O-O-O Na6 11. Rhe1 Nc7</t>
+  </si>
+  <si>
+    <t>1. e4 e5 2. Nf3 Nf6 3. Nxe5 d6 4. Nf3 Nxe4 5. Nc3 Nxc3 6. dxc3 Be7 7. Be3 O-O 8. Qd2 Nc6 9. O-O-O Ne5 10. Kb1 Re8 11. Nd4 a6</t>
+  </si>
+  <si>
+    <t>1. e4 e5 2. Nf3 Nf6 3. d4 Nxe4 4. Bd3 d5 5. Nxe5 Nd7 6. Nxd7 Bxd7 7. O-O Qh4 8. c4 O-O-O 9. c5 g5 10. Nc3 Bg7 11. g3 Qh3</t>
+  </si>
+  <si>
+    <t>1. e4 e5 2. Nf3 Nf6 3. d4 Nxe4 4. Bd3 d5 5. Nxe5 Bd6 6. O-O O-O 7. c4 Bxe5 8. dxe5 Nc6 9. cxd5 Qxd5 10. Qc2 Nb4 11. Bxe4 Nxc2</t>
+  </si>
+  <si>
+    <t>1. e4 e5 2. Nf3 Nf6 3. d4 Nxe4 4. Bd3 Nc6 5. Bxe4 d5 6. Bg5 Qd7 7. Bd3 e4 8. O-O f6 9. Bf4 exd3 10. Qxd3 Bd6 11. Re1+ Kf7</t>
+  </si>
+  <si>
+    <t>1. e4 e5 2. Nf3 Nf6 3. d4 exd4 4. e5 Ne4 5. Qxd4 d5 6. exd6 Nxd6 7. Nc3 Nc6 8. Qf4 g6 9. Be3 Bg7 10. O-O-O O-O 11. h4 h6</t>
   </si>
 </sst>
 </file>
@@ -853,6 +996,14 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1622,6 +1773,156 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="30.57"/>
+    <col customWidth="1" min="2" max="2" width="122.57"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="30.57"/>
+    <col customWidth="1" min="2" max="2" width="161.71"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -2460,44 +2761,244 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+      <c r="A10" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+      <c r="A11" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
+      <c r="A12" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+      <c r="A13" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+      <c r="A14" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+      <c r="A15" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+      <c r="A16" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2528,50 +3029,50 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>184</v>
+        <v>216</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>185</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>184</v>
+        <v>216</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>186</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>184</v>
+        <v>216</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>187</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>184</v>
+        <v>216</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>188</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>184</v>
+        <v>216</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>189</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>184</v>
+        <v>216</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>190</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -2603,66 +3104,66 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>191</v>
+        <v>223</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>192</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>191</v>
+        <v>223</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>193</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>191</v>
+        <v>223</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>194</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>195</v>
+        <v>227</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>196</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>195</v>
+        <v>227</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>197</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>198</v>
+        <v>230</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>199</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>198</v>
+        <v>230</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>200</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>198</v>
+        <v>230</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>201</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -2694,378 +3195,378 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>202</v>
+        <v>234</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>203</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>202</v>
+        <v>234</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>204</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>202</v>
+        <v>234</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>205</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>202</v>
+        <v>234</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>206</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>202</v>
+        <v>234</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>207</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>208</v>
+        <v>234</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>209</v>
+        <v>234</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>210</v>
+        <v>234</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>211</v>
+        <v>234</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>212</v>
+        <v>234</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>213</v>
+        <v>234</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>214</v>
+        <v>234</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>215</v>
+        <v>234</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>216</v>
+        <v>234</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>217</v>
+        <v>234</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>218</v>
+        <v>234</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>219</v>
+        <v>234</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>220</v>
+        <v>234</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>221</v>
+        <v>234</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>222</v>
+        <v>234</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>223</v>
+        <v>234</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>224</v>
+        <v>234</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>202</v>
+        <v>234</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>225</v>
+        <v>257</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>202</v>
+        <v>234</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>226</v>
+        <v>258</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>227</v>
+        <v>234</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>228</v>
+        <v>234</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>229</v>
+        <v>234</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>230</v>
+        <v>234</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>231</v>
+        <v>234</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>233</v>
+      <c r="A31" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>234</v>
+      <c r="A32" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>235</v>
+      <c r="A33" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>236</v>
+      <c r="A34" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>237</v>
+      <c r="A35" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>238</v>
+      <c r="A36" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>240</v>
+      <c r="A37" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>241</v>
+      <c r="A38" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>242</v>
+      <c r="A39" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>243</v>
+      <c r="A40" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>244</v>
+      <c r="A41" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>245</v>
+      <c r="A42" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>246</v>
+      <c r="A43" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>247</v>
+      <c r="A44" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>248</v>
+      <c r="A45" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>249</v>
+      <c r="A46" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>250</v>
+      <c r="A47" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>251</v>
+      <c r="A48" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -3095,6 +3596,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>